<commit_message>
parser succes read from file
</commit_message>
<xml_diff>
--- a/RN16_learn/trial02/RN16.xlsx
+++ b/RN16_learn/trial02/RN16.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A170FC-4E8A-4FDB-909C-686DA0CC832C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBCF6A44-22A8-476E-B7B9-2F75D3FC2443}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7417,10 +7417,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B255ED-1049-4732-9347-9184B1A874F9}">
-  <dimension ref="B1:D131"/>
+  <dimension ref="B1:E131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T36" sqref="F2:T36"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7429,7 +7429,7 @@
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7440,17 +7440,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>0.253585</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0.253554</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>0.253687</v>
       </c>
@@ -7462,8 +7462,12 @@
         <f>IF(AND((B4&gt;C4),(ABS(B4-C4)&gt;0.001)), 0.28, 0.25)</f>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <f>IF(AND(($B4&gt;$C4),(ABS($B4-$C4)&gt;0.001)), 1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>0.25370999999999999</v>
       </c>
@@ -7475,1643 +7479,2151 @@
         <f t="shared" ref="D5:D68" si="0">IF(AND((B5&gt;C5),(ABS(B5-C5)&gt;0.001)), 0.28, 0.25)</f>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <f t="shared" ref="E5:E68" si="1">IF(AND(($B5&gt;$C5),(ABS($B5-$C5)&gt;0.001)), 1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>0.253577</v>
       </c>
       <c r="C6">
-        <f t="shared" ref="C6:C69" si="1">C5*0.8 + B6*0.2</f>
+        <f t="shared" ref="C6:C69" si="2">C5*0.8 + B6*0.2</f>
         <v>0.25361854666666667</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>0.25363599999999997</v>
       </c>
       <c r="C7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25362203733333333</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>0.25360199999999999</v>
       </c>
       <c r="C8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25361802986666671</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>0.25361800000000001</v>
       </c>
       <c r="C9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25361802389333338</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>0.25366</v>
       </c>
       <c r="C10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25362641911466671</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>0.25366100000000003</v>
       </c>
       <c r="C11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25363333529173337</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>0.25353199999999998</v>
       </c>
       <c r="C12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.2536130682333867</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>0.25358599999999998</v>
       </c>
       <c r="C13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25360765458670936</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>0.25340600000000002</v>
       </c>
       <c r="C14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25356732366936752</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>0.25393300000000002</v>
       </c>
       <c r="C15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25364045893549403</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>0.25289499999999998</v>
       </c>
       <c r="C16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25349136714839521</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>0.257386</v>
       </c>
       <c r="C17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25427029371871618</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>0.275057</v>
       </c>
       <c r="C18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25842763497497295</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>0.276559</v>
       </c>
       <c r="C19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26205390797997841</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>0.27459499999999998</v>
       </c>
       <c r="C20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26456212638398274</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>0.25526300000000002</v>
       </c>
       <c r="C21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26270230110718618</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>0.25884099999999999</v>
       </c>
       <c r="C22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26193004088574895</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>0.27796500000000002</v>
       </c>
       <c r="C23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26513703270859917</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>0.26173000000000002</v>
       </c>
       <c r="C24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26445562616687934</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>0.25222299999999997</v>
       </c>
       <c r="C25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26200910093350349</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>0.252747</v>
       </c>
       <c r="C26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26015668074680282</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>0.26227200000000001</v>
       </c>
       <c r="C27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26057974459744226</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>0.27757700000000002</v>
       </c>
       <c r="C28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.2639791956779538</v>
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>0.25879799999999997</v>
       </c>
       <c r="C29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26294295654236305</v>
       </c>
       <c r="D29">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>0.252272</v>
       </c>
       <c r="C30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26080876523389046</v>
       </c>
       <c r="D30">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>0.25370399999999999</v>
       </c>
       <c r="C31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25938781218711238</v>
       </c>
       <c r="D31">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>0.25306899999999999</v>
       </c>
       <c r="C32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25812404974968989</v>
       </c>
       <c r="D32">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>0.25464700000000001</v>
       </c>
       <c r="C33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25742863979975195</v>
       </c>
       <c r="D33">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>0.27254899999999999</v>
       </c>
       <c r="C34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26045271183980157</v>
       </c>
       <c r="D34">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>0.27668700000000002</v>
       </c>
       <c r="C35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26369956947184126</v>
       </c>
       <c r="D35">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>0.27615499999999998</v>
       </c>
       <c r="C36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26619065557747301</v>
       </c>
       <c r="D36">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>0.25940000000000002</v>
       </c>
       <c r="C37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26483252446197847</v>
       </c>
       <c r="D37">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>0.25489699999999998</v>
       </c>
       <c r="C38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26284541956958279</v>
       </c>
       <c r="D38">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>0.27616000000000002</v>
       </c>
       <c r="C39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26550833565566623</v>
       </c>
       <c r="D39">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>0.26700200000000002</v>
       </c>
       <c r="C40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26580706852453301</v>
       </c>
       <c r="D40">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>0.25102200000000002</v>
       </c>
       <c r="C41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26285005481962642</v>
       </c>
       <c r="D41">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>0.27040700000000001</v>
       </c>
       <c r="C42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26436144385570115</v>
       </c>
       <c r="D42">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>0.27136399999999999</v>
       </c>
       <c r="C43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26576195508456091</v>
       </c>
       <c r="D43">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>0.25132599999999999</v>
       </c>
       <c r="C44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26287476406764876</v>
       </c>
       <c r="D44">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>0.266069</v>
       </c>
       <c r="C45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26351361125411898</v>
       </c>
       <c r="D45">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>0.27649400000000002</v>
       </c>
       <c r="C46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26610968900329524</v>
       </c>
       <c r="D46">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>0.25551099999999999</v>
       </c>
       <c r="C47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26398995120263619</v>
       </c>
       <c r="D47">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>0.25813900000000001</v>
       </c>
       <c r="C48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26281976096210896</v>
       </c>
       <c r="D48">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>0.27678000000000003</v>
       </c>
       <c r="C49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26561180876968721</v>
       </c>
       <c r="D49">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>0.25939400000000001</v>
       </c>
       <c r="C50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26436824701574979</v>
       </c>
       <c r="D50">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>0.252502</v>
       </c>
       <c r="C51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26199499761259981</v>
       </c>
       <c r="D51">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>0.25226900000000002</v>
       </c>
       <c r="C52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26004979809007989</v>
       </c>
       <c r="D52">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>0.26205200000000001</v>
       </c>
       <c r="C53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26045023847206394</v>
       </c>
       <c r="D53">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>0.27695900000000001</v>
       </c>
       <c r="C54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26375199077765116</v>
       </c>
       <c r="D54">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E54">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>0.27632000000000001</v>
       </c>
       <c r="C55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26626559262212091</v>
       </c>
       <c r="D55">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E55">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>0.27062399999999998</v>
       </c>
       <c r="C56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26713727409769672</v>
       </c>
       <c r="D56">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E56">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>0.25143500000000002</v>
       </c>
       <c r="C57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26399681927815738</v>
       </c>
       <c r="D57">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E57">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>0.26569599999999999</v>
       </c>
       <c r="C58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26433665542252593</v>
       </c>
       <c r="D58">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E58">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>0.27650000000000002</v>
       </c>
       <c r="C59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26676932433802075</v>
       </c>
       <c r="D59">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>0.25624200000000003</v>
       </c>
       <c r="C60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26466385947041665</v>
       </c>
       <c r="D60">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E60">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>0.25309799999999999</v>
       </c>
       <c r="C61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26235068757633334</v>
       </c>
       <c r="D61">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>0.25203199999999998</v>
       </c>
       <c r="C62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26028695006106667</v>
       </c>
       <c r="D62">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E62">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>0.26552300000000001</v>
       </c>
       <c r="C63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26133416004885335</v>
       </c>
       <c r="D63">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>0.27714699999999998</v>
       </c>
       <c r="C64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.2644967280390827</v>
       </c>
       <c r="D64">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>0.27668199999999998</v>
       </c>
       <c r="C65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26693378243126614</v>
       </c>
       <c r="D65">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>0.27026699999999998</v>
       </c>
       <c r="C66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26760042594501293</v>
       </c>
       <c r="D66">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E66">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67">
         <v>0.25269999999999998</v>
       </c>
       <c r="C67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26462034075601037</v>
       </c>
       <c r="D67">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68">
         <v>0.25307299999999999</v>
       </c>
       <c r="C68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26231087260480829</v>
       </c>
       <c r="D68">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E68">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69">
         <v>0.25595499999999999</v>
       </c>
       <c r="C69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26103969808384664</v>
       </c>
       <c r="D69">
-        <f t="shared" ref="D69:D131" si="2">IF(AND((B69&gt;C69),(ABS(B69-C69)&gt;0.001)), 0.28, 0.25)</f>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D69:D131" si="3">IF(AND((B69&gt;C69),(ABS(B69-C69)&gt;0.001)), 0.28, 0.25)</f>
+        <v>0.25</v>
+      </c>
+      <c r="E69">
+        <f t="shared" ref="E69:E131" si="4">IF(AND(($B69&gt;$C69),(ABS($B69-$C69)&gt;0.001)), 1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70">
         <v>0.27453699999999998</v>
       </c>
       <c r="C70">
-        <f t="shared" ref="C70:C131" si="3">C69*0.8 + B70*0.2</f>
+        <f t="shared" ref="C70:C131" si="5">C69*0.8 + B70*0.2</f>
         <v>0.26373915846707729</v>
       </c>
       <c r="D70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E70">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71">
         <v>0.27633000000000002</v>
       </c>
       <c r="C71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26625732677366187</v>
       </c>
       <c r="D71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E71">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72">
         <v>0.27679900000000002</v>
       </c>
       <c r="C72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26836566141892954</v>
       </c>
       <c r="D72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E72">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B73">
         <v>0.26000800000000002</v>
       </c>
       <c r="C73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26669412913514368</v>
       </c>
       <c r="D73">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74">
         <v>0.25216699999999997</v>
       </c>
       <c r="C74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26378870330811494</v>
       </c>
       <c r="D74">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B75">
         <v>0.252888</v>
       </c>
       <c r="C75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26160856264649196</v>
       </c>
       <c r="D75">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76">
         <v>0.26481900000000003</v>
       </c>
       <c r="C76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26225065011719362</v>
       </c>
       <c r="D76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E76">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77">
         <v>0.277418</v>
       </c>
       <c r="C77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.2652841200937549</v>
       </c>
       <c r="D77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E77">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B78">
         <v>0.255907</v>
       </c>
       <c r="C78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26340869607500395</v>
       </c>
       <c r="D78">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B79">
         <v>0.25807600000000003</v>
       </c>
       <c r="C79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26234215686000317</v>
       </c>
       <c r="D79">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B80">
         <v>0.27608500000000002</v>
       </c>
       <c r="C80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26509072548800255</v>
       </c>
       <c r="D80">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E80">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>0.27648699999999998</v>
       </c>
       <c r="C81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26736998039040205</v>
       </c>
       <c r="D81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E81">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82">
         <v>0.27360499999999999</v>
       </c>
       <c r="C82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26861698431232167</v>
       </c>
       <c r="D82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E82">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>0.25457099999999999</v>
       </c>
       <c r="C83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26580778744985734</v>
       </c>
       <c r="D83">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84">
         <v>0.25356899999999999</v>
       </c>
       <c r="C84">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26336002995988589</v>
       </c>
       <c r="D84">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85">
         <v>0.25304399999999999</v>
       </c>
       <c r="C85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26129682396790871</v>
       </c>
       <c r="D85">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B86">
         <v>0.268455</v>
       </c>
       <c r="C86">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26272845917432697</v>
       </c>
       <c r="D86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E86">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B87">
         <v>0.27541199999999999</v>
       </c>
       <c r="C87">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26526516733946159</v>
       </c>
       <c r="D87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E87">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B88">
         <v>0.25332700000000002</v>
       </c>
       <c r="C88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26287753387156931</v>
       </c>
       <c r="D88">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B89">
         <v>0.26150200000000001</v>
       </c>
       <c r="C89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26260242709725545</v>
       </c>
       <c r="D89">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90">
         <v>0.27686899999999998</v>
       </c>
       <c r="C90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26545574167780439</v>
       </c>
       <c r="D90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E90">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B91">
         <v>0.27639599999999998</v>
       </c>
       <c r="C91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26764379334224353</v>
       </c>
       <c r="D91">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E91">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92">
         <v>0.27361999999999997</v>
       </c>
       <c r="C92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26883903467379483</v>
       </c>
       <c r="D92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E92">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B93">
         <v>0.254716</v>
       </c>
       <c r="C93">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26601442773903589</v>
       </c>
       <c r="D93">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B94">
         <v>0.25283499999999998</v>
       </c>
       <c r="C94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26337854219122869</v>
       </c>
       <c r="D94">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B95">
         <v>0.253496</v>
       </c>
       <c r="C95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26140203375298299</v>
       </c>
       <c r="D95">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B96">
         <v>0.25332700000000002</v>
       </c>
       <c r="C96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25978702700238643</v>
       </c>
       <c r="D96">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E96">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B97">
         <v>0.253446</v>
       </c>
       <c r="C97">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25851882160190914</v>
       </c>
       <c r="D97">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E97">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B98">
         <v>0.25339699999999998</v>
       </c>
       <c r="C98">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25749445728152731</v>
       </c>
       <c r="D98">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B99">
         <v>0.25353100000000001</v>
       </c>
       <c r="C99">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25670176582522186</v>
       </c>
       <c r="D99">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E99">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B100">
         <v>0.25347599999999998</v>
       </c>
       <c r="C100">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25605661266017749</v>
       </c>
       <c r="D100">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E100">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B101">
         <v>0.25346800000000003</v>
       </c>
       <c r="C101">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25553889012814202</v>
       </c>
       <c r="D101">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E101">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B102">
         <v>0.25356699999999999</v>
       </c>
       <c r="C102">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25514451210251365</v>
       </c>
       <c r="D102">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E102">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B103">
         <v>0.25353500000000001</v>
       </c>
       <c r="C103">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25482260968201093</v>
       </c>
       <c r="D103">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E103">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B104">
         <v>0.25346800000000003</v>
       </c>
       <c r="C104">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25455168774560877</v>
       </c>
       <c r="D104">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E104">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B105">
         <v>0.25359999999999999</v>
       </c>
       <c r="C105">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25436135019648703</v>
       </c>
       <c r="D105">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E105">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B106">
         <v>0.25350800000000001</v>
       </c>
       <c r="C106">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25419068015718965</v>
       </c>
       <c r="D106">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E106">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B107">
         <v>0.25349899999999997</v>
       </c>
       <c r="C107">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25405234412575173</v>
       </c>
       <c r="D107">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E107">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B108">
         <v>0.25361099999999998</v>
       </c>
       <c r="C108">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25396407530060139</v>
       </c>
       <c r="D108">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E108">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B109">
         <v>0.25363000000000002</v>
       </c>
       <c r="C109">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25389726024048115</v>
       </c>
       <c r="D109">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E109">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B110">
         <v>0.25357000000000002</v>
       </c>
       <c r="C110">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25383180819238493</v>
       </c>
       <c r="D110">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E110">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B111">
         <v>0.25361400000000001</v>
       </c>
       <c r="C111">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25378824655390797</v>
       </c>
       <c r="D111">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E111">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B112">
         <v>0.25341599999999997</v>
       </c>
       <c r="C112">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25371379724312637</v>
       </c>
       <c r="D112">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E112">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B113">
         <v>0.253444</v>
       </c>
       <c r="C113">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25365983779450108</v>
       </c>
       <c r="D113">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E113">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B114">
         <v>0.25348399999999999</v>
       </c>
       <c r="C114">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25362467023560087</v>
       </c>
       <c r="D114">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E114">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B115">
         <v>0.25344899999999998</v>
       </c>
       <c r="C115">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25358953618848068</v>
       </c>
       <c r="D115">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E115">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B116">
         <v>0.25347399999999998</v>
       </c>
       <c r="C116">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25356642895078457</v>
       </c>
       <c r="D116">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E116">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B117">
         <v>0.25350499999999998</v>
       </c>
       <c r="C117">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25355414316062763</v>
       </c>
       <c r="D117">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E117">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B118">
         <v>0.25337999999999999</v>
       </c>
       <c r="C118">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25351931452850213</v>
       </c>
       <c r="D118">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E118">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B119">
         <v>0.25337199999999999</v>
       </c>
       <c r="C119">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25348985162280169</v>
       </c>
       <c r="D119">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E119">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B120">
         <v>0.25336399999999998</v>
       </c>
       <c r="C120">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25346468129824135</v>
       </c>
       <c r="D120">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E120">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B121">
         <v>0.25342700000000001</v>
       </c>
       <c r="C121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25345714503859307</v>
       </c>
       <c r="D121">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E121">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B122">
         <v>0.25343399999999999</v>
       </c>
       <c r="C122">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25345251603087449</v>
       </c>
       <c r="D122">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E122">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B123">
         <v>0.25346800000000003</v>
       </c>
       <c r="C123">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25345561282469964</v>
       </c>
       <c r="D123">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E123">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B124">
         <v>0.25343500000000002</v>
       </c>
       <c r="C124">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25345149025975977</v>
       </c>
       <c r="D124">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E124">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B125">
         <v>0.25345400000000001</v>
       </c>
       <c r="C125">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25345199220780784</v>
       </c>
       <c r="D125">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E125">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B126">
         <v>0.25351400000000002</v>
       </c>
       <c r="C126">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.2534643937662463</v>
       </c>
       <c r="D126">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E126">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B127">
         <v>0.25334000000000001</v>
       </c>
       <c r="C127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25343951501299705</v>
       </c>
       <c r="D127">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E127">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B128">
         <v>0.25350400000000001</v>
       </c>
       <c r="C128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25345241201039764</v>
       </c>
       <c r="D128">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E128">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B129">
         <v>0.25348300000000001</v>
       </c>
       <c r="C129">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25345852960831816</v>
       </c>
       <c r="D129">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E129">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B130">
         <v>0.25341799999999998</v>
       </c>
       <c r="C130">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25345042368665455</v>
       </c>
       <c r="D130">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E130">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B131">
         <v>0.253492</v>
       </c>
       <c r="C131">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25345873894932369</v>
       </c>
       <c r="D131">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="E131">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>